<commit_message>
added confusion matrices and F1 thrsholds
</commit_message>
<xml_diff>
--- a/data/CCIP-RT-02 eDNA data.xlsx
+++ b/data/CCIP-RT-02 eDNA data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smatthew\Documents\GitKraken\CCIP-eDNA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121DCADC-39B5-43FF-9574-3CB9940D56AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BFEB78-C205-4665-8A2E-F707C589FE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{29985091-A0C7-4C6D-AF6E-9D175D7CC9B7}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{29985091-A0C7-4C6D-AF6E-9D175D7CC9B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -953,14 +953,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D821CED7-4F6A-4204-B6D6-9FE74BF10085}">
   <dimension ref="A1:S649"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A605" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>